<commit_message>
major update including redone boundary - trying to fix one cell problem
</commit_message>
<xml_diff>
--- a/Data/Data_geology/bore_data_Otorowiri.xlsx
+++ b/Data/Data_geology/bore_data_Otorowiri.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="strat (2)" sheetId="1" state="visible" r:id="rId1"/>
@@ -60,6 +60,7 @@
     </font>
     <font>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -627,9 +628,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.453125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -887,10 +888,10 @@
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20.1796875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.1796875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="20.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3841,12 +3842,12 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.453125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3983,10 +3984,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="30" t="n">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="K3" s="29" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="L3" s="29" t="n">
         <v>0.0001</v>
@@ -4109,10 +4110,10 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20.1796875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.1796875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="20.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7066,9 +7067,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.7265625" customWidth="1" min="1" max="1"/>
+    <col width="9.7109375" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
confinement added and some transience
</commit_message>
<xml_diff>
--- a/Data/Data_geology/bore_data_Otorowiri.xlsx
+++ b/Data/Data_geology/bore_data_Otorowiri.xlsx
@@ -13110,7 +13110,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>128</v>
+        <v>129.7204895019531</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -13152,7 +13152,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>128</v>
+        <v>129.7204895019531</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -13189,7 +13189,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>107</v>
+        <v>105.2605514526367</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -13258,7 +13258,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>107</v>
+        <v>105.2605514526367</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -13295,7 +13295,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>148</v>
+        <v>148.1514434814453</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -13337,7 +13337,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>148</v>
+        <v>148.1514434814453</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -13374,7 +13374,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>220</v>
+        <v>221.2654418945312</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -13428,7 +13428,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>139</v>
+        <v>139.1471862792969</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -13473,7 +13473,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>139</v>
+        <v>139.1471862792969</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -13510,7 +13510,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>123</v>
+        <v>116.8295288085938</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -13579,7 +13579,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>123</v>
+        <v>116.8295288085938</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -13616,7 +13616,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>193</v>
+        <v>206.3394927978516</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -13658,7 +13658,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>193</v>
+        <v>206.3394927978516</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -13695,7 +13695,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>201</v>
+        <v>201.3811798095703</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -13737,7 +13737,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>201</v>
+        <v>201.3811798095703</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -13774,7 +13774,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>241</v>
+        <v>240.5259704589844</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -13834,7 +13834,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>241</v>
+        <v>240.5259704589844</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -13871,7 +13871,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>233</v>
+        <v>231.5464019775391</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -13934,7 +13934,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>233</v>
+        <v>231.5464019775391</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -13977,7 +13977,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>258</v>
+        <v>257.8213195800781</v>
       </c>
       <c r="G21" t="n">
         <v>25</v>
@@ -14015,7 +14015,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>258</v>
+        <v>259.987060546875</v>
       </c>
       <c r="G22" t="n">
         <v>85</v>
@@ -14053,7 +14053,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>169</v>
+        <v>168.0024566650391</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -14095,7 +14095,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>169</v>
+        <v>168.0024566650391</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -14132,7 +14132,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>254</v>
+        <v>256.0364990234375</v>
       </c>
       <c r="G25" t="n">
         <v>216</v>
@@ -14170,7 +14170,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>203</v>
+        <v>193.2759399414062</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -14210,7 +14210,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>203</v>
+        <v>193.2759399414062</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -14249,7 +14249,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>222</v>
+        <v>223.0767211914062</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -14289,7 +14289,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>222</v>
+        <v>223.0767211914062</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -14328,7 +14328,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>276</v>
+        <v>279.4418029785156</v>
       </c>
       <c r="G30" t="n">
         <v>94</v>
@@ -14366,7 +14366,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>184</v>
+        <v>210.6910400390625</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -14408,7 +14408,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>184</v>
+        <v>210.6910400390625</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -14445,7 +14445,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>283</v>
+        <v>284.1803588867188</v>
       </c>
       <c r="G33" t="n">
         <v>183</v>
@@ -14483,7 +14483,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>267</v>
+        <v>268.218994140625</v>
       </c>
       <c r="G34" t="n">
         <v>159</v>
@@ -14521,7 +14521,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>265</v>
+        <v>265.193115234375</v>
       </c>
       <c r="G35" t="n">
         <v>247</v>
@@ -14560,7 +14560,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>208</v>
+        <v>210.8645935058594</v>
       </c>
       <c r="G36" t="n">
         <v>183</v>
@@ -14599,7 +14599,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>218</v>
+        <v>216.2009887695312</v>
       </c>
       <c r="G37" t="n">
         <v>152</v>
@@ -14638,7 +14638,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>306</v>
+        <v>307.6929626464844</v>
       </c>
       <c r="G38" t="n">
         <v>204</v>
@@ -14675,7 +14675,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>272</v>
+        <v>272.0730590820312</v>
       </c>
       <c r="G39" t="n">
         <v>195</v>
@@ -14712,7 +14712,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>227</v>
+        <v>226.4542846679688</v>
       </c>
       <c r="G40" t="n">
         <v>195</v>
@@ -14751,7 +14751,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>222</v>
+        <v>223.0819702148438</v>
       </c>
       <c r="G41" t="n">
         <v>137</v>
@@ -14790,7 +14790,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>209</v>
+        <v>211.1378479003906</v>
       </c>
       <c r="G42" t="n">
         <v>167</v>
@@ -14827,7 +14827,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>299</v>
+        <v>299.9042053222656</v>
       </c>
       <c r="G43" t="n">
         <v>199</v>
@@ -14865,7 +14865,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>295</v>
+        <v>295.7376098632812</v>
       </c>
       <c r="G44" t="n">
         <v>434</v>
@@ -14903,7 +14903,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>311</v>
+        <v>308.8829956054688</v>
       </c>
       <c r="G45" t="n">
         <v>107</v>
@@ -14941,7 +14941,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>222</v>
+        <v>223.0211029052734</v>
       </c>
       <c r="G46" t="n">
         <v>110</v>
@@ -14980,7 +14980,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>256</v>
+        <v>226.7249450683594</v>
       </c>
       <c r="G47" t="n">
         <v>102</v>
@@ -15019,7 +15019,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>231</v>
+        <v>233.7315521240234</v>
       </c>
       <c r="G48" t="n">
         <v>158</v>
@@ -15058,7 +15058,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>228</v>
+        <v>228.9816436767578</v>
       </c>
       <c r="G49" t="n">
         <v>107</v>
@@ -15097,7 +15097,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>280</v>
+        <v>276.9217224121094</v>
       </c>
       <c r="G50" t="n">
         <v>302</v>
@@ -15136,7 +15136,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>266</v>
+        <v>267.8984680175781</v>
       </c>
       <c r="G51" t="n">
         <v>140</v>
@@ -15175,7 +15175,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>288</v>
+        <v>288.9960021972656</v>
       </c>
       <c r="G52" t="n">
         <v>299</v>
@@ -15214,7 +15214,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>264</v>
+        <v>265.5480041503906</v>
       </c>
       <c r="G53" t="n">
         <v>378</v>
@@ -15252,7 +15252,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>280</v>
+        <v>281.3111877441406</v>
       </c>
       <c r="G54" t="n">
         <v>70</v>
@@ -15291,7 +15291,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>281</v>
+        <v>282.0736694335938</v>
       </c>
       <c r="G55" t="n">
         <v>105</v>
@@ -15330,7 +15330,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>257</v>
+        <v>258.8345336914062</v>
       </c>
       <c r="G56" t="n">
         <v>291</v>
@@ -15368,7 +15368,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>276</v>
+        <v>271.9231262207031</v>
       </c>
       <c r="G57" t="n">
         <v>55</v>
@@ -15403,7 +15403,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>220</v>
+        <v>221.2654418945312</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -19246,7 +19246,7 @@
         <v>6701564</v>
       </c>
       <c r="D2" t="n">
-        <v>201</v>
+        <v>201.3811798095703</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -19289,7 +19289,7 @@
         <v>6701564</v>
       </c>
       <c r="D3" t="n">
-        <v>201</v>
+        <v>201.3811798095703</v>
       </c>
       <c r="E3" t="n">
         <v>124</v>
@@ -19326,7 +19326,7 @@
         <v>6701564</v>
       </c>
       <c r="D4" t="n">
-        <v>201</v>
+        <v>201.3811798095703</v>
       </c>
       <c r="E4" t="n">
         <v>100</v>
@@ -19363,7 +19363,7 @@
         <v>6749507</v>
       </c>
       <c r="D5" t="n">
-        <v>241</v>
+        <v>240.5259704589844</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -19406,7 +19406,7 @@
         <v>6749507</v>
       </c>
       <c r="D6" t="n">
-        <v>241</v>
+        <v>240.5259704589844</v>
       </c>
       <c r="E6" t="n">
         <v>124</v>
@@ -19443,7 +19443,7 @@
         <v>6749507</v>
       </c>
       <c r="D7" t="n">
-        <v>241</v>
+        <v>240.5259704589844</v>
       </c>
       <c r="E7" t="n">
         <v>100</v>
@@ -19480,7 +19480,7 @@
         <v>6749291</v>
       </c>
       <c r="D8" t="n">
-        <v>233</v>
+        <v>231.5464019775391</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -19523,7 +19523,7 @@
         <v>6749291</v>
       </c>
       <c r="D9" t="n">
-        <v>233</v>
+        <v>231.5464019775391</v>
       </c>
       <c r="E9" t="n">
         <v>124</v>
@@ -19560,7 +19560,7 @@
         <v>6749291</v>
       </c>
       <c r="D10" t="n">
-        <v>233</v>
+        <v>231.5464019775391</v>
       </c>
       <c r="E10" t="n">
         <v>100</v>
@@ -19597,7 +19597,7 @@
         <v>6752754</v>
       </c>
       <c r="D11" t="n">
-        <v>258</v>
+        <v>257.8213195800781</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -19640,7 +19640,7 @@
         <v>6752754</v>
       </c>
       <c r="D12" t="n">
-        <v>233</v>
+        <v>232.8213195800781</v>
       </c>
       <c r="E12" t="n">
         <v>124</v>
@@ -19677,7 +19677,7 @@
         <v>6752754</v>
       </c>
       <c r="D13" t="n">
-        <v>168</v>
+        <v>167.8213195800781</v>
       </c>
       <c r="E13" t="n">
         <v>100</v>
@@ -19714,7 +19714,7 @@
         <v>6746453</v>
       </c>
       <c r="D14" t="n">
-        <v>258</v>
+        <v>259.987060546875</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -19757,7 +19757,7 @@
         <v>6746453</v>
       </c>
       <c r="D15" t="n">
-        <v>173</v>
+        <v>174.987060546875</v>
       </c>
       <c r="E15" t="n">
         <v>124</v>
@@ -19794,7 +19794,7 @@
         <v>6746453</v>
       </c>
       <c r="D16" t="n">
-        <v>121</v>
+        <v>122.987060546875</v>
       </c>
       <c r="E16" t="n">
         <v>100</v>
@@ -19831,7 +19831,7 @@
         <v>6736093</v>
       </c>
       <c r="D17" t="n">
-        <v>169</v>
+        <v>168.0024566650391</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -19874,7 +19874,7 @@
         <v>6736093</v>
       </c>
       <c r="D18" t="n">
-        <v>169</v>
+        <v>168.0024566650391</v>
       </c>
       <c r="E18" t="n">
         <v>124</v>
@@ -19911,7 +19911,7 @@
         <v>6736093</v>
       </c>
       <c r="D19" t="n">
-        <v>169</v>
+        <v>168.0024566650391</v>
       </c>
       <c r="E19" t="n">
         <v>100</v>
@@ -19948,7 +19948,7 @@
         <v>6702012</v>
       </c>
       <c r="D20" t="n">
-        <v>254</v>
+        <v>256.0364990234375</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -19991,7 +19991,7 @@
         <v>6702012</v>
       </c>
       <c r="D21" t="n">
-        <v>38</v>
+        <v>40.0364990234375</v>
       </c>
       <c r="E21" t="n">
         <v>124</v>
@@ -20028,7 +20028,7 @@
         <v>6702012</v>
       </c>
       <c r="D22" t="n">
-        <v>-42</v>
+        <v>-39.9635009765625</v>
       </c>
       <c r="E22" t="n">
         <v>100</v>
@@ -20065,7 +20065,7 @@
         <v>6739317</v>
       </c>
       <c r="D23" t="n">
-        <v>203</v>
+        <v>193.2759399414062</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -20108,7 +20108,7 @@
         <v>6739317</v>
       </c>
       <c r="D24" t="n">
-        <v>172</v>
+        <v>162.2759399414062</v>
       </c>
       <c r="E24" t="n">
         <v>100</v>
@@ -20145,7 +20145,7 @@
         <v>6739317</v>
       </c>
       <c r="D25" t="n">
-        <v>203</v>
+        <v>193.2759399414062</v>
       </c>
       <c r="E25" t="n">
         <v>124</v>
@@ -20182,7 +20182,7 @@
         <v>6740261</v>
       </c>
       <c r="D26" t="n">
-        <v>222</v>
+        <v>223.0767211914062</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -20225,7 +20225,7 @@
         <v>6740261</v>
       </c>
       <c r="D27" t="n">
-        <v>155</v>
+        <v>156.0767211914062</v>
       </c>
       <c r="E27" t="n">
         <v>100</v>
@@ -20262,7 +20262,7 @@
         <v>6740261</v>
       </c>
       <c r="D28" t="n">
-        <v>222</v>
+        <v>223.0767211914062</v>
       </c>
       <c r="E28" t="n">
         <v>124</v>
@@ -20299,7 +20299,7 @@
         <v>6743138</v>
       </c>
       <c r="D29" t="n">
-        <v>276</v>
+        <v>279.4418029785156</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -20342,7 +20342,7 @@
         <v>6743138</v>
       </c>
       <c r="D30" t="n">
-        <v>182</v>
+        <v>185.4418029785156</v>
       </c>
       <c r="E30" t="n">
         <v>124</v>
@@ -20379,7 +20379,7 @@
         <v>6743138</v>
       </c>
       <c r="D31" t="n">
-        <v>127</v>
+        <v>130.4418029785156</v>
       </c>
       <c r="E31" t="n">
         <v>100</v>
@@ -20416,7 +20416,7 @@
         <v>6735088</v>
       </c>
       <c r="D32" t="n">
-        <v>184</v>
+        <v>210.6910400390625</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -20459,7 +20459,7 @@
         <v>6735088</v>
       </c>
       <c r="D33" t="n">
-        <v>184</v>
+        <v>210.6910400390625</v>
       </c>
       <c r="E33" t="n">
         <v>124</v>
@@ -20496,7 +20496,7 @@
         <v>6735088</v>
       </c>
       <c r="D34" t="n">
-        <v>184</v>
+        <v>210.6910400390625</v>
       </c>
       <c r="E34" t="n">
         <v>100</v>
@@ -20533,7 +20533,7 @@
         <v>6744727</v>
       </c>
       <c r="D35" t="n">
-        <v>283</v>
+        <v>284.1803588867188</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -20576,7 +20576,7 @@
         <v>6744727</v>
       </c>
       <c r="D36" t="n">
-        <v>100</v>
+        <v>101.1803588867188</v>
       </c>
       <c r="E36" t="n">
         <v>124</v>
@@ -20613,7 +20613,7 @@
         <v>6744727</v>
       </c>
       <c r="D37" t="n">
-        <v>42</v>
+        <v>43.18035888671881</v>
       </c>
       <c r="E37" t="n">
         <v>100</v>
@@ -20650,7 +20650,7 @@
         <v>6747056</v>
       </c>
       <c r="D38" t="n">
-        <v>267</v>
+        <v>268.218994140625</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -20693,7 +20693,7 @@
         <v>6747056</v>
       </c>
       <c r="D39" t="n">
-        <v>108</v>
+        <v>109.218994140625</v>
       </c>
       <c r="E39" t="n">
         <v>124</v>
@@ -20730,7 +20730,7 @@
         <v>6747056</v>
       </c>
       <c r="D40" t="n">
-        <v>38</v>
+        <v>39.218994140625</v>
       </c>
       <c r="E40" t="n">
         <v>100</v>
@@ -20767,7 +20767,7 @@
         <v>6742933</v>
       </c>
       <c r="D41" t="n">
-        <v>265</v>
+        <v>265.193115234375</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -20810,7 +20810,7 @@
         <v>6742933</v>
       </c>
       <c r="D42" t="n">
-        <v>18</v>
+        <v>18.193115234375</v>
       </c>
       <c r="E42" t="n">
         <v>124</v>
@@ -20847,7 +20847,7 @@
         <v>6741005</v>
       </c>
       <c r="D43" t="n">
-        <v>208</v>
+        <v>210.8645935058594</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -20890,7 +20890,7 @@
         <v>6741005</v>
       </c>
       <c r="D44" t="n">
-        <v>25</v>
+        <v>27.8645935058594</v>
       </c>
       <c r="E44" t="n">
         <v>124</v>
@@ -20927,7 +20927,7 @@
         <v>6739238</v>
       </c>
       <c r="D45" t="n">
-        <v>218</v>
+        <v>216.2009887695312</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -20970,7 +20970,7 @@
         <v>6739238</v>
       </c>
       <c r="D46" t="n">
-        <v>66</v>
+        <v>64.20098876953119</v>
       </c>
       <c r="E46" t="n">
         <v>124</v>
@@ -21007,7 +21007,7 @@
         <v>6732904</v>
       </c>
       <c r="D47" t="n">
-        <v>306</v>
+        <v>307.6929626464844</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -21050,7 +21050,7 @@
         <v>6732904</v>
       </c>
       <c r="D48" t="n">
-        <v>102</v>
+        <v>103.6929626464844</v>
       </c>
       <c r="E48" t="n">
         <v>124</v>
@@ -21087,7 +21087,7 @@
         <v>6732904</v>
       </c>
       <c r="D49" t="n">
-        <v>70</v>
+        <v>71.69296264648438</v>
       </c>
       <c r="E49" t="n">
         <v>100</v>
@@ -21124,7 +21124,7 @@
         <v>6737076</v>
       </c>
       <c r="D50" t="n">
-        <v>272</v>
+        <v>272.0730590820312</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -21167,7 +21167,7 @@
         <v>6737076</v>
       </c>
       <c r="D51" t="n">
-        <v>77</v>
+        <v>77.07305908203119</v>
       </c>
       <c r="E51" t="n">
         <v>124</v>
@@ -21204,7 +21204,7 @@
         <v>6737076</v>
       </c>
       <c r="D52" t="n">
-        <v>50</v>
+        <v>50.07305908203119</v>
       </c>
       <c r="E52" t="n">
         <v>100</v>
@@ -21241,7 +21241,7 @@
         <v>6739543</v>
       </c>
       <c r="D53" t="n">
-        <v>227</v>
+        <v>226.4542846679688</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -21284,7 +21284,7 @@
         <v>6739543</v>
       </c>
       <c r="D54" t="n">
-        <v>32</v>
+        <v>31.45428466796881</v>
       </c>
       <c r="E54" t="n">
         <v>124</v>
@@ -21321,7 +21321,7 @@
         <v>6741138</v>
       </c>
       <c r="D55" t="n">
-        <v>222</v>
+        <v>223.0819702148438</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -21364,7 +21364,7 @@
         <v>6741138</v>
       </c>
       <c r="D56" t="n">
-        <v>85</v>
+        <v>86.08197021484381</v>
       </c>
       <c r="E56" t="n">
         <v>124</v>
@@ -21401,7 +21401,7 @@
         <v>6740424</v>
       </c>
       <c r="D57" t="n">
-        <v>209</v>
+        <v>211.1378479003906</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -21444,7 +21444,7 @@
         <v>6740424</v>
       </c>
       <c r="D58" t="n">
-        <v>42</v>
+        <v>44.1378479003906</v>
       </c>
       <c r="E58" t="n">
         <v>124</v>
@@ -21481,7 +21481,7 @@
         <v>6740424</v>
       </c>
       <c r="D59" t="n">
-        <v>15</v>
+        <v>17.1378479003906</v>
       </c>
       <c r="E59" t="n">
         <v>100</v>
@@ -21518,7 +21518,7 @@
         <v>6752577</v>
       </c>
       <c r="D60" t="n">
-        <v>299</v>
+        <v>299.9042053222656</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -21561,7 +21561,7 @@
         <v>6752577</v>
       </c>
       <c r="D61" t="n">
-        <v>100</v>
+        <v>100.9042053222656</v>
       </c>
       <c r="E61" t="n">
         <v>124</v>
@@ -21598,7 +21598,7 @@
         <v>6752577</v>
       </c>
       <c r="D62" t="n">
-        <v>70</v>
+        <v>70.90420532226562</v>
       </c>
       <c r="E62" t="n">
         <v>100</v>
@@ -21635,7 +21635,7 @@
         <v>6702360</v>
       </c>
       <c r="D63" t="n">
-        <v>295</v>
+        <v>295.7376098632812</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -21678,7 +21678,7 @@
         <v>6702360</v>
       </c>
       <c r="D64" t="n">
-        <v>-139</v>
+        <v>-138.2623901367188</v>
       </c>
       <c r="E64" t="n">
         <v>124</v>
@@ -21715,7 +21715,7 @@
         <v>6702360</v>
       </c>
       <c r="D65" t="n">
-        <v>-233</v>
+        <v>-232.2623901367188</v>
       </c>
       <c r="E65" t="n">
         <v>100</v>
@@ -21752,7 +21752,7 @@
         <v>6730642</v>
       </c>
       <c r="D66" t="n">
-        <v>311</v>
+        <v>308.8829956054688</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -21795,7 +21795,7 @@
         <v>6730642</v>
       </c>
       <c r="D67" t="n">
-        <v>204</v>
+        <v>201.8829956054688</v>
       </c>
       <c r="E67" t="n">
         <v>124</v>
@@ -21832,7 +21832,7 @@
         <v>6730642</v>
       </c>
       <c r="D68" t="n">
-        <v>36</v>
+        <v>33.88299560546881</v>
       </c>
       <c r="E68" t="n">
         <v>100</v>
@@ -21869,7 +21869,7 @@
         <v>6738631</v>
       </c>
       <c r="D69" t="n">
-        <v>222</v>
+        <v>223.0211029052734</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -21912,7 +21912,7 @@
         <v>6738631</v>
       </c>
       <c r="D70" t="n">
-        <v>112</v>
+        <v>113.0211029052734</v>
       </c>
       <c r="E70" t="n">
         <v>124</v>
@@ -21949,7 +21949,7 @@
         <v>6742469</v>
       </c>
       <c r="D71" t="n">
-        <v>256</v>
+        <v>226.7249450683594</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -21992,7 +21992,7 @@
         <v>6742469</v>
       </c>
       <c r="D72" t="n">
-        <v>154</v>
+        <v>124.7249450683594</v>
       </c>
       <c r="E72" t="n">
         <v>124</v>
@@ -22029,7 +22029,7 @@
         <v>6735766</v>
       </c>
       <c r="D73" t="n">
-        <v>231</v>
+        <v>233.7315521240234</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
@@ -22072,7 +22072,7 @@
         <v>6735766</v>
       </c>
       <c r="D74" t="n">
-        <v>73</v>
+        <v>75.73155212402341</v>
       </c>
       <c r="E74" t="n">
         <v>124</v>
@@ -22109,7 +22109,7 @@
         <v>6739524</v>
       </c>
       <c r="D75" t="n">
-        <v>228</v>
+        <v>228.9816436767578</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
@@ -22152,7 +22152,7 @@
         <v>6739524</v>
       </c>
       <c r="D76" t="n">
-        <v>121</v>
+        <v>121.9816436767578</v>
       </c>
       <c r="E76" t="n">
         <v>124</v>
@@ -22189,7 +22189,7 @@
         <v>6720858</v>
       </c>
       <c r="D77" t="n">
-        <v>280</v>
+        <v>276.9217224121094</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -22232,7 +22232,7 @@
         <v>6720858</v>
       </c>
       <c r="D78" t="n">
-        <v>-22</v>
+        <v>-25.07827758789062</v>
       </c>
       <c r="E78" t="n">
         <v>124</v>
@@ -22269,7 +22269,7 @@
         <v>6731712</v>
       </c>
       <c r="D79" t="n">
-        <v>288</v>
+        <v>288.9960021972656</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -22312,7 +22312,7 @@
         <v>6731712</v>
       </c>
       <c r="D80" t="n">
-        <v>-11</v>
+        <v>-10.00399780273438</v>
       </c>
       <c r="E80" t="n">
         <v>124</v>
@@ -22349,7 +22349,7 @@
         <v>6702687</v>
       </c>
       <c r="D81" t="n">
-        <v>264</v>
+        <v>265.5480041503906</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -22392,7 +22392,7 @@
         <v>6702687</v>
       </c>
       <c r="D82" t="n">
-        <v>-114</v>
+        <v>-112.4519958496094</v>
       </c>
       <c r="E82" t="n">
         <v>124</v>
@@ -22429,7 +22429,7 @@
         <v>6702687</v>
       </c>
       <c r="D83" t="n">
-        <v>-216</v>
+        <v>-214.4519958496094</v>
       </c>
       <c r="E83" t="n">
         <v>100</v>
@@ -22466,7 +22466,7 @@
         <v>6695215</v>
       </c>
       <c r="D84" t="n">
-        <v>280</v>
+        <v>281.3111877441406</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -22509,7 +22509,7 @@
         <v>6695215</v>
       </c>
       <c r="D85" t="n">
-        <v>210</v>
+        <v>211.3111877441406</v>
       </c>
       <c r="E85" t="n">
         <v>124</v>
@@ -22546,7 +22546,7 @@
         <v>6695161</v>
       </c>
       <c r="D86" t="n">
-        <v>281</v>
+        <v>282.0736694335938</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -22589,7 +22589,7 @@
         <v>6695161</v>
       </c>
       <c r="D87" t="n">
-        <v>176</v>
+        <v>177.0736694335938</v>
       </c>
       <c r="E87" t="n">
         <v>124</v>
@@ -22626,7 +22626,7 @@
         <v>6702762</v>
       </c>
       <c r="D88" t="n">
-        <v>257</v>
+        <v>258.8345336914062</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -22669,7 +22669,7 @@
         <v>6702762</v>
       </c>
       <c r="D89" t="n">
-        <v>-34</v>
+        <v>-32.16546630859381</v>
       </c>
       <c r="E89" t="n">
         <v>124</v>
@@ -22706,7 +22706,7 @@
         <v>6702762</v>
       </c>
       <c r="D90" t="n">
-        <v>-100</v>
+        <v>-98.16546630859381</v>
       </c>
       <c r="E90" t="n">
         <v>100</v>

</xml_diff>